<commit_message>
Change descrip in xlsx file for IISBMP2, add export table for appendix
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/S2_BMP_summary_select.xlsx
+++ b/experiments/IISBMP2/data/S2_BMP_summary_select.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="S2_BMP_summary_select" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterate="1" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -60,10 +60,10 @@
     <t>Cellulose</t>
   </si>
   <si>
-    <t>Substrate C</t>
-  </si>
-  <si>
-    <t>Substrate D</t>
+    <t>FIC</t>
+  </si>
+  <si>
+    <t>LBD</t>
   </si>
 </sst>
 </file>

</xml_diff>